<commit_message>
Se actualiza el archivo original de excel
</commit_message>
<xml_diff>
--- a/ExternalAssets/Language.xlsx
+++ b/ExternalAssets/Language.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Oiden\OneDrive\Documentos\ProyectosUnity\plantilla\ExternalAssets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{134B448C-39EB-4118-AB53-AED8B3590D39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84B23CA7-5D1F-4098-858B-A0BFFA95EF72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="39">
   <si>
     <t>ID</t>
   </si>
@@ -47,9 +47,6 @@
     <t>English</t>
   </si>
   <si>
-    <t>Spanish</t>
-  </si>
-  <si>
     <t>Play</t>
   </si>
   <si>
@@ -117,6 +114,45 @@
   </si>
   <si>
     <t>General</t>
+  </si>
+  <si>
+    <t>OptionText: TitleLanguage</t>
+  </si>
+  <si>
+    <t>Language</t>
+  </si>
+  <si>
+    <t>Lenguaje</t>
+  </si>
+  <si>
+    <t>OptionButton: BackButtonText</t>
+  </si>
+  <si>
+    <t>Back</t>
+  </si>
+  <si>
+    <t>Atrás</t>
+  </si>
+  <si>
+    <t>OptionButton: HomeButtonText</t>
+  </si>
+  <si>
+    <t>Home</t>
+  </si>
+  <si>
+    <t>Inicio</t>
+  </si>
+  <si>
+    <t>OptionButton: TitleResolutionMute</t>
+  </si>
+  <si>
+    <t>FullScreen</t>
+  </si>
+  <si>
+    <t>Pantalla Completa</t>
+  </si>
+  <si>
+    <t>Español</t>
   </si>
 </sst>
 </file>
@@ -522,7 +558,7 @@
   <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -545,7 +581,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -553,13 +589,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
         <v>4</v>
-      </c>
-      <c r="D2" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -567,13 +603,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
         <v>6</v>
-      </c>
-      <c r="D3" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -581,13 +617,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
         <v>8</v>
-      </c>
-      <c r="D4" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -595,13 +631,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" t="s">
         <v>6</v>
-      </c>
-      <c r="D5" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -609,13 +645,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
         <v>14</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>15</v>
-      </c>
-      <c r="D6" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -623,13 +659,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -637,13 +673,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -651,13 +687,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -665,27 +701,71 @@
         <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" t="s">
         <v>24</v>
-      </c>
-      <c r="D10" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
+      <c r="B11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" t="s">
+        <v>28</v>
+      </c>
       <c r="G11" s="2"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C12" s="4"/>
-      <c r="D12" s="1"/>
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B13" s="1"/>
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D18" s="5"/>

</xml_diff>